<commit_message>
update 1 file and create 1 file
</commit_message>
<xml_diff>
--- a/TrackerFile.xlsx
+++ b/TrackerFile.xlsx
@@ -1,67 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pai.suryadarshan/Desktop/Minions (Bots)/BOTS ;D/2024-25/Tracker/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB910FEB-B79C-5C4C-A92F-88008FF38D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Blender" sheetId="1" r:id="rId1"/>
-    <sheet name="ML" sheetId="2" r:id="rId2"/>
-    <sheet name="Read (Academic)" sheetId="3" r:id="rId3"/>
-    <sheet name="Read (Non-Academic)" sheetId="4" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blender" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ML" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Read (Academic)" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Read (Non-Academic)" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="6">
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Desc. (Opt)</t>
-  </si>
-  <si>
-    <t>Sign-in</t>
-  </si>
-  <si>
-    <t>Sign-out</t>
-  </si>
-  <si>
-    <t>Time Spent</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[hh]:mm:ss"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -80,12 +51,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -185,68 +156,128 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table0" displayName="Table13456" ref="A1:E2" insertRow="1" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
-  <autoFilter ref="A1:E2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table0" displayName="Table13456" ref="A1:E2" headerRowCount="1" insertRow="1" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="A1:E2"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Desc. (Opt)" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Sign-in" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Sign-out" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Time Spent" dataDxfId="21"/>
+    <tableColumn id="1" name="Date" dataDxfId="25"/>
+    <tableColumn id="6" name="Desc. (Opt)" dataDxfId="24"/>
+    <tableColumn id="3" name="Sign-in" dataDxfId="23"/>
+    <tableColumn id="5" name="Sign-out" dataDxfId="22"/>
+    <tableColumn id="2" name="Time Spent" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table134542" ref="A1:E2" insertRow="1" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
-  <autoFilter ref="A1:E2" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table1" displayName="Table134542" ref="A1:E2" headerRowCount="1" insertRow="1" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+  <autoFilter ref="A1:E2"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Date" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Desc. (Opt)" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Sign-in" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Sign-out" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Time Spent" dataDxfId="14"/>
+    <tableColumn id="1" name="Date" dataDxfId="18"/>
+    <tableColumn id="6" name="Desc. (Opt)" dataDxfId="17"/>
+    <tableColumn id="3" name="Sign-in" dataDxfId="16"/>
+    <tableColumn id="5" name="Sign-out" dataDxfId="15"/>
+    <tableColumn id="2" name="Time Spent" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table2" displayName="Table1345" ref="A1:E2" insertRow="1" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:E2" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table2" displayName="Table1345" ref="A1:E2" headerRowCount="1" insertRow="1" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A1:E2"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Date" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Desc. (Opt)" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Sign-in" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Sign-out" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Time Spent" dataDxfId="7"/>
+    <tableColumn id="1" name="Date" dataDxfId="11"/>
+    <tableColumn id="6" name="Desc. (Opt)" dataDxfId="10"/>
+    <tableColumn id="3" name="Sign-in" dataDxfId="9"/>
+    <tableColumn id="5" name="Sign-out" dataDxfId="8"/>
+    <tableColumn id="2" name="Time Spent" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table13454" displayName="Table13454" ref="A1:E2" insertRow="1" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E2" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table3" displayName="Table13454" ref="A1:E3" headerRowCount="1" insertRow="1" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E2"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Date" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Desc. (Opt)" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Sign-in" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Sign-out" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Time Spent" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" dataDxfId="4"/>
+    <tableColumn id="6" name="Desc. (Opt)" dataDxfId="3"/>
+    <tableColumn id="3" name="Sign-in" dataDxfId="2"/>
+    <tableColumn id="5" name="Sign-out" dataDxfId="1"/>
+    <tableColumn id="2" name="Time Spent" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -568,191 +599,249 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" customWidth="1"/>
-    <col min="2" max="2" width="43.83203125" customWidth="1"/>
-    <col min="4" max="5" width="14.5" customWidth="1"/>
-    <col min="6" max="6" width="44" customWidth="1"/>
+    <col width="12.83203125" customWidth="1" min="1" max="1"/>
+    <col width="43.83203125" customWidth="1" min="2" max="2"/>
+    <col width="14.5" customWidth="1" min="4" max="5"/>
+    <col width="44" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Desc. (Opt)</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Sign-in</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Sign-out</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Time Spent</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E2" s="3"/>
+    <row r="2">
+      <c r="E2" s="3" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" customWidth="1"/>
-    <col min="2" max="2" width="43.83203125" customWidth="1"/>
-    <col min="4" max="5" width="14.5" customWidth="1"/>
-    <col min="6" max="6" width="44" customWidth="1"/>
+    <col width="12.83203125" customWidth="1" min="1" max="1"/>
+    <col width="43.83203125" customWidth="1" min="2" max="2"/>
+    <col width="14.5" customWidth="1" min="4" max="5"/>
+    <col width="44" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Desc. (Opt)</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Sign-in</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Sign-out</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Time Spent</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E2" s="1"/>
+    <row r="2">
+      <c r="E2" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" customWidth="1"/>
-    <col min="2" max="2" width="43.83203125" customWidth="1"/>
-    <col min="3" max="4" width="14.5" customWidth="1"/>
+    <col width="12.83203125" customWidth="1" min="1" max="1"/>
+    <col width="43.83203125" customWidth="1" min="2" max="2"/>
+    <col width="14.5" customWidth="1" min="3" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Desc. (Opt)</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Sign-in</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Sign-out</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Time Spent</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E2" s="1"/>
+    <row r="2">
+      <c r="E2" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:J9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" customWidth="1"/>
-    <col min="2" max="2" width="43.83203125" customWidth="1"/>
-    <col min="4" max="5" width="14.5" customWidth="1"/>
-    <col min="6" max="6" width="44" customWidth="1"/>
+    <col width="12.83203125" customWidth="1" min="1" max="1"/>
+    <col width="43.83203125" customWidth="1" min="2" max="2"/>
+    <col width="14.5" customWidth="1" min="4" max="5"/>
+    <col width="44" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Desc. (Opt)</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Sign-in</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Sign-out</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Time Spent</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J3" s="2"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="H5" s="2"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="H9" t="s">
-        <v>5</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>03/12/24</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>12:14</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>12:37</t>
+        </is>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>0.01597222222222222</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update P1_Append_Times_to_sheet.py, TrackerFile.xlsx and P1_Append_Times_to_sheet.cpython-39.pyc
</commit_message>
<xml_diff>
--- a/TrackerFile.xlsx
+++ b/TrackerFile.xlsx
@@ -256,7 +256,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table2" displayName="Table1345" ref="A1:E2" headerRowCount="1" insertRow="1" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table2" displayName="Table1345" ref="A1:E3" headerRowCount="1" insertRow="1" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A1:E2"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Date" dataDxfId="11"/>
@@ -761,7 +761,24 @@
       </c>
     </row>
     <row r="2">
-      <c r="E2" s="1" t="n"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>03/12/24</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>12:41</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>12:48</t>
+        </is>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>0.004861111111111111</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update 0_Main.py and TrackerFile.xlsx
</commit_message>
<xml_diff>
--- a/TrackerFile.xlsx
+++ b/TrackerFile.xlsx
@@ -228,7 +228,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table0" displayName="Table13456" ref="A1:E2" headerRowCount="1" insertRow="1" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table0" displayName="Table13456" ref="A1:E3" headerRowCount="1" insertRow="1" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="A1:E2"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Date" dataDxfId="25"/>
@@ -242,7 +242,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table1" displayName="Table134542" ref="A1:E3" headerRowCount="1" insertRow="1" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table1" displayName="Table134542" ref="A1:E4" headerRowCount="1" insertRow="1" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A1:E2"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Date" dataDxfId="18"/>
@@ -270,7 +270,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table3" displayName="Table13454" ref="A1:E3" headerRowCount="1" insertRow="1" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table3" displayName="Table13454" ref="A1:E5" headerRowCount="1" insertRow="1" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:E2"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Date" dataDxfId="4"/>
@@ -646,7 +646,24 @@
       </c>
     </row>
     <row r="2">
-      <c r="E2" s="3" t="n"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>03/12/24</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>21:56</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>22:51</t>
+        </is>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>0.03819444444444445</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -662,7 +679,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E2"/>
@@ -709,14 +726,39 @@
           <t>03/12/24</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
           <t>14:09</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>16:40</t>
+        </is>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>0.1048611111111111</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>05/12/24</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>10:34</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>10:54</t>
+        </is>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>0.01388888888888889</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -806,7 +848,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E2"/>
@@ -867,6 +909,46 @@
         <v>0.01597222222222222</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>04/12/24</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>10:50</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>13:07</t>
+        </is>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>0.09513888888888888</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>05/12/24</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>10:36</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>10:55</t>
+        </is>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>0.01319444444444444</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>